<commit_message>
Base state from Sara with updated template
</commit_message>
<xml_diff>
--- a/CostingSheetTemplate.xlsx
+++ b/CostingSheetTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\nrb-costing-sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\costing-sheets-com\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79A05600-6C8A-488E-A8AE-0AA0852DA0D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C555B252-B3A3-4966-9FD7-D631015188C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="55">
   <si>
     <t>Boat #</t>
   </si>
@@ -184,9 +184,6 @@
   </si>
   <si>
     <t xml:space="preserve">TOTAL ENGINE &amp; JET </t>
-  </si>
-  <si>
-    <t>Engine - Jet</t>
   </si>
   <si>
     <t>Canvas Materials</t>
@@ -1277,9 +1274,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:J461"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1947,7 +1942,7 @@
         <v>46</v>
       </c>
       <c r="I35" s="71">
-        <f>SUM(I8:I34)*0.08</f>
+        <f>SUM(I6:I34)*0</f>
         <v>0</v>
       </c>
       <c r="J35" s="23"/>
@@ -1958,7 +1953,7 @@
         <v>10</v>
       </c>
       <c r="I36" s="54">
-        <f>SUM(I8:I34)+I35</f>
+        <f>SUM(I6:I34)+I35</f>
         <v>0</v>
       </c>
       <c r="J36" s="23"/>
@@ -2629,7 +2624,7 @@
         <v>46</v>
       </c>
       <c r="I67" s="10">
-        <f>SUM(I42:I66)*0.5</f>
+        <f>SUM(I40:I66)*0</f>
         <v>0</v>
       </c>
       <c r="J67" s="23"/>
@@ -2640,7 +2635,7 @@
         <v>13</v>
       </c>
       <c r="I68" s="54">
-        <f>SUM(I42:I66)+I67</f>
+        <f>SUM(I40:I66)+I67</f>
         <v>0</v>
       </c>
       <c r="J68" s="23"/>
@@ -2667,7 +2662,7 @@
         <v>11</v>
       </c>
       <c r="C71" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H71" s="13"/>
       <c r="I71" s="15"/>
@@ -3320,10 +3315,10 @@
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C100" s="14"/>
       <c r="H100" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I100" s="54">
-        <f>SUM(I74:I98)</f>
+        <f>SUM(I73:I98)</f>
         <v>0</v>
       </c>
       <c r="J100" s="23"/>
@@ -9036,7 +9031,7 @@
         <v>19</v>
       </c>
       <c r="I363" s="25">
-        <f>SUM(I106:I361)</f>
+        <f>SUM(I105:I361)</f>
         <v>0</v>
       </c>
       <c r="J363"/>
@@ -9354,7 +9349,7 @@
     <row r="385" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D385" s="34"/>
       <c r="H385" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I385" s="6">
         <f>I383+I373+I363</f>
@@ -9825,7 +9820,7 @@
     </row>
     <row r="419" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D419" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I419" s="25">
         <f>I100</f>
@@ -9853,7 +9848,7 @@
     </row>
     <row r="422" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D422" s="34" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G422" s="25"/>
       <c r="H422" s="9"/>
@@ -9868,7 +9863,7 @@
         <v>29</v>
       </c>
       <c r="I423" s="6">
-        <f>SUM(I417:I421)</f>
+        <f>SUM(I417:I422)</f>
         <v>0</v>
       </c>
     </row>
@@ -9895,7 +9890,7 @@
         <v>56.69</v>
       </c>
       <c r="I428" s="25">
-        <f>G428*F428</f>
+        <f t="shared" ref="I428:I433" si="28">G428*F428</f>
         <v>0</v>
       </c>
     </row>
@@ -9908,15 +9903,22 @@
         <v>30.22</v>
       </c>
       <c r="I429" s="25">
-        <f>G429*F429</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
     <row r="430" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D430" s="34"/>
+      <c r="D430" s="34" t="s">
+        <v>53</v>
+      </c>
       <c r="F430" s="14"/>
-      <c r="G430" s="75"/>
-      <c r="I430" s="25"/>
+      <c r="G430" s="75">
+        <v>0</v>
+      </c>
+      <c r="I430" s="25">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="431" spans="3:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D431" s="34" t="s">
@@ -9927,7 +9929,7 @@
         <v>35.619999999999997</v>
       </c>
       <c r="I431" s="25">
-        <f>G431*F431</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
@@ -9940,7 +9942,7 @@
         <v>40.840000000000003</v>
       </c>
       <c r="I432" s="25">
-        <f>G432*F432</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
@@ -9953,7 +9955,7 @@
         <v>36</v>
       </c>
       <c r="I433" s="25">
-        <f>G433*F433</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>